<commit_message>
send msg to each page
</commit_message>
<xml_diff>
--- a/doc/命令.xlsx
+++ b/doc/命令.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="3" lowestEdited="5" rupBuild="9302"/>
   <workbookPr/>
   <bookViews>
-    <workbookView windowWidth="23280" windowHeight="10350" activeTab="2"/>
+    <workbookView windowWidth="19380" windowHeight="10350" activeTab="2"/>
   </bookViews>
   <sheets>
     <sheet name="快捷方式" sheetId="1" r:id="rId1"/>
@@ -80,10 +80,10 @@
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <numFmts count="4">
+    <numFmt numFmtId="43" formatCode="_ * #,##0.00_ ;_ * \-#,##0.00_ ;_ * &quot;-&quot;??_ ;_ @_ "/>
+    <numFmt numFmtId="44" formatCode="_ &quot;￥&quot;* #,##0.00_ ;_ &quot;￥&quot;* \-#,##0.00_ ;_ &quot;￥&quot;* &quot;-&quot;??_ ;_ @_ "/>
+    <numFmt numFmtId="42" formatCode="_ &quot;￥&quot;* #,##0_ ;_ &quot;￥&quot;* \-#,##0_ ;_ &quot;￥&quot;* &quot;-&quot;_ ;_ @_ "/>
     <numFmt numFmtId="41" formatCode="_ * #,##0_ ;_ * \-#,##0_ ;_ * &quot;-&quot;_ ;_ @_ "/>
-    <numFmt numFmtId="43" formatCode="_ * #,##0.00_ ;_ * \-#,##0.00_ ;_ * &quot;-&quot;??_ ;_ @_ "/>
-    <numFmt numFmtId="42" formatCode="_ &quot;￥&quot;* #,##0_ ;_ &quot;￥&quot;* \-#,##0_ ;_ &quot;￥&quot;* &quot;-&quot;_ ;_ @_ "/>
-    <numFmt numFmtId="44" formatCode="_ &quot;￥&quot;* #,##0.00_ ;_ &quot;￥&quot;* \-#,##0.00_ ;_ &quot;￥&quot;* &quot;-&quot;??_ ;_ @_ "/>
   </numFmts>
   <fonts count="24">
     <font>
@@ -191,6 +191,59 @@
       <scheme val="minor"/>
     </font>
     <font>
+      <sz val="11"/>
+      <color rgb="FF9C6500"/>
+      <name val="宋体"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF3F3F76"/>
+      <name val="宋体"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color rgb="FFFA7D00"/>
+      <name val="宋体"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FFFA7D00"/>
+      <name val="宋体"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="宋体"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="18"/>
+      <color theme="3"/>
+      <name val="宋体"/>
+      <charset val="134"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <u/>
+      <sz val="11"/>
+      <color rgb="FF0000FF"/>
+      <name val="宋体"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
       <b/>
       <sz val="11"/>
       <color rgb="FF3F3F3F"/>
@@ -208,59 +261,6 @@
     </font>
     <font>
       <sz val="11"/>
-      <color rgb="FF9C6500"/>
-      <name val="宋体"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FF3F3F76"/>
-      <name val="宋体"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="11"/>
-      <color rgb="FFFA7D00"/>
-      <name val="宋体"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FFFA7D00"/>
-      <name val="宋体"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="11"/>
-      <color theme="1"/>
-      <name val="宋体"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="18"/>
-      <color theme="3"/>
-      <name val="宋体"/>
-      <charset val="134"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <u/>
-      <sz val="11"/>
-      <color rgb="FF0000FF"/>
-      <name val="宋体"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
       <color rgb="FF006100"/>
       <name val="宋体"/>
       <charset val="0"/>
@@ -324,6 +324,96 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFEB9C"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFCC99"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFF2F2F2"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
         <fgColor theme="8"/>
         <bgColor indexed="64"/>
       </patternFill>
@@ -342,97 +432,7 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor rgb="FFF2F2F2"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
         <fgColor rgb="FFFFFFCC"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFEB9C"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFCC99"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -490,36 +490,6 @@
       <top/>
       <bottom style="medium">
         <color theme="4"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="thin">
-        <color rgb="FF3F3F3F"/>
-      </left>
-      <right style="thin">
-        <color rgb="FF3F3F3F"/>
-      </right>
-      <top style="thin">
-        <color rgb="FF3F3F3F"/>
-      </top>
-      <bottom style="thin">
-        <color rgb="FF3F3F3F"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="thin">
-        <color rgb="FFB2B2B2"/>
-      </left>
-      <right style="thin">
-        <color rgb="FFB2B2B2"/>
-      </right>
-      <top style="thin">
-        <color rgb="FFB2B2B2"/>
-      </top>
-      <bottom style="thin">
-        <color rgb="FFB2B2B2"/>
       </bottom>
       <diagonal/>
     </border>
@@ -567,6 +537,36 @@
       </bottom>
       <diagonal/>
     </border>
+    <border>
+      <left style="thin">
+        <color rgb="FF3F3F3F"/>
+      </left>
+      <right style="thin">
+        <color rgb="FF3F3F3F"/>
+      </right>
+      <top style="thin">
+        <color rgb="FF3F3F3F"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="FF3F3F3F"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color rgb="FFB2B2B2"/>
+      </left>
+      <right style="thin">
+        <color rgb="FFB2B2B2"/>
+      </right>
+      <top style="thin">
+        <color rgb="FFB2B2B2"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="FFB2B2B2"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="49">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0">
@@ -575,10 +575,10 @@
     <xf numFmtId="42" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="5" fillId="22" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="17" fillId="19" borderId="5" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="5" fillId="18" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="15" fillId="14" borderId="3" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="44" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
@@ -596,124 +596,124 @@
     <xf numFmtId="43" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="13" fillId="21" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="20" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="9" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="28" borderId="8" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="13" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="19" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="22" fillId="0" borderId="2" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="2" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="20" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="6" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="12" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="21" fillId="17" borderId="7" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="16" fillId="17" borderId="3" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="8" borderId="1" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="24" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="17" fillId="0" borderId="4" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="18" fillId="0" borderId="5" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="23" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="11" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="16" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="27" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="15" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="7" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="30" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="4" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="26" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="23" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="29" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="3" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="13" fillId="25" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="22" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="9" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="14" borderId="4" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="18" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="21" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="15" fillId="0" borderId="2" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="0" borderId="2" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="24" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="8" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="17" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="14" fillId="13" borderId="3" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="18" fillId="13" borderId="5" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="8" borderId="1" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="28" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="19" fillId="0" borderId="6" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="20" fillId="0" borderId="7" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="23" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="16" fillId="16" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="21" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="12" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="20" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="7" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="30" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="4" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="11" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="27" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="29" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="3" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="5" fillId="6" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="19" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="22" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="2" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="13" fillId="10" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="6" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="23" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="26" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="2" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="15" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
   </cellStyleXfs>
@@ -1674,6 +1674,90 @@
         <a:xfrm>
           <a:off x="0" y="87268050"/>
           <a:ext cx="9714230" cy="4914265"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:noFill/>
+        <a:ln w="9525">
+          <a:noFill/>
+        </a:ln>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>0</xdr:col>
+      <xdr:colOff>0</xdr:colOff>
+      <xdr:row>540</xdr:row>
+      <xdr:rowOff>0</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>13</xdr:col>
+      <xdr:colOff>303530</xdr:colOff>
+      <xdr:row>559</xdr:row>
+      <xdr:rowOff>94615</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="22" name="图片 21"/>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip r:embed="rId21"/>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="0" y="92583000"/>
+          <a:ext cx="9218930" cy="3352165"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:noFill/>
+        <a:ln w="9525">
+          <a:noFill/>
+        </a:ln>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>0</xdr:col>
+      <xdr:colOff>0</xdr:colOff>
+      <xdr:row>561</xdr:row>
+      <xdr:rowOff>0</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>13</xdr:col>
+      <xdr:colOff>332105</xdr:colOff>
+      <xdr:row>591</xdr:row>
+      <xdr:rowOff>46990</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="23" name="图片 22"/>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip r:embed="rId22"/>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="0" y="96183450"/>
+          <a:ext cx="9247505" cy="5190490"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -2121,8 +2205,8 @@
   <sheetPr/>
   <dimension ref="A171:O319"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A484" workbookViewId="0">
-      <selection activeCell="A510" sqref="A510"/>
+    <sheetView tabSelected="1" topLeftCell="A541" workbookViewId="0">
+      <selection activeCell="A562" sqref="A562"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9" defaultRowHeight="13.5"/>

</xml_diff>